<commit_message>
Added species and legacy columns to main script tibble. Added Shorok's graph script.
</commit_message>
<xml_diff>
--- a/Writing Progress Tracker.xlsx
+++ b/Writing Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB88F364-88AD-4410-AB31-984CB510BD26}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE30E4F3-0ACB-48C5-9395-9A9A5AF79479}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" activeTab="1" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
   </bookViews>
   <sheets>
     <sheet name="Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -123,8 +123,8 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1792,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB62B3D-6049-438B-9FF7-BB33F44B353D}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12557BC7-E9BB-4FF3-ACB5-C0458929F97B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated vectors to 1-8stressor designs, added a power test that I don't understand
</commit_message>
<xml_diff>
--- a/Writing Progress Tracker.xlsx
+++ b/Writing Progress Tracker.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE30E4F3-0ACB-48C5-9395-9A9A5AF79479}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC459FED-A288-4769-8D33-D5AFBF1F1071}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" activeTab="2" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
   </bookViews>
   <sheets>
     <sheet name="Spreadsheet" sheetId="1" r:id="rId1"/>
     <sheet name="Chart" sheetId="3" r:id="rId2"/>
+    <sheet name="Papers List" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Day</t>
   </si>
@@ -53,6 +54,207 @@
   </si>
   <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Date Published</t>
+  </si>
+  <si>
+    <t>Date Found</t>
+  </si>
+  <si>
+    <t>Date Reviewed</t>
+  </si>
+  <si>
+    <t>Annual Review of Ecology, Evolution, and Systematics</t>
+  </si>
+  <si>
+    <t>Tom Bell</t>
+  </si>
+  <si>
+    <t>D. Tilman, F. Isbell, J. Cowles</t>
+  </si>
+  <si>
+    <t>Reconceptualizing synergism and antagonism among multiple stressors</t>
+  </si>
+  <si>
+    <t>Ecology and Evolution</t>
+  </si>
+  <si>
+    <t>J. Pigott, C. Townsend, C. Matthaei</t>
+  </si>
+  <si>
+    <t>Mendely</t>
+  </si>
+  <si>
+    <t>Compounded Perturbations Yield Ecological Surprises</t>
+  </si>
+  <si>
+    <t>Ecosystems</t>
+  </si>
+  <si>
+    <t>R. Paine, M. Tegner, E. Johnson</t>
+  </si>
+  <si>
+    <t>Synergism and antagonism among multiple stressors</t>
+  </si>
+  <si>
+    <t>Limonology and Oceanography</t>
+  </si>
+  <si>
+    <t>C. Folt, C. Chen, M. Moore, J. Burnaford</t>
+  </si>
+  <si>
+    <t>Interactive and cumulative effects of multiple human stressors in marine systems</t>
+  </si>
+  <si>
+    <t>Ecology Letters</t>
+  </si>
+  <si>
+    <t>C. Crain, K. Kroeker, B. Halpern</t>
+  </si>
+  <si>
+    <t>Chapter Twelve - Recommendations for the Next Generation of Global Freshwater Biological Monitoring Tools</t>
+  </si>
+  <si>
+    <t>Advances in Ecological Research</t>
+  </si>
+  <si>
+    <t>Jackson, Pigott, Woodward, etc.</t>
+  </si>
+  <si>
+    <t>Climate warming and agricultural stressors interact to determine stream periphyton community composition</t>
+  </si>
+  <si>
+    <t>Global Change Biology</t>
+  </si>
+  <si>
+    <t>Pigott, Salis, Lear, Townsend, Matthaei</t>
+  </si>
+  <si>
+    <t>FORUM: Ecological networks: the missing links in biomonitoring science</t>
+  </si>
+  <si>
+    <t>Journal of Applied Biology</t>
+  </si>
+  <si>
+    <t>Gray, Gorman, Woodward</t>
+  </si>
+  <si>
+    <t>Multiple anthropogenic stressors and the structural properties of food webs</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E. O'Gorman, J. Fitch, T. Crowe </t>
+  </si>
+  <si>
+    <t>Net effects of multiple stressors in freshwater ecosystems: a meta‐analysis</t>
+  </si>
+  <si>
+    <t>M. Jackson, C. Loewen, R. Vinebrooke, C. Chimimba</t>
+  </si>
+  <si>
+    <t>Fostering integration of freshwater ecology with ecotoxicology</t>
+  </si>
+  <si>
+    <t>Freshwater Biology</t>
+  </si>
+  <si>
+    <t>M. Gessner, A. Tlili</t>
+  </si>
+  <si>
+    <t>Advancing understanding and prediction in multiple stressor research through a mechanistic basis for null models</t>
+  </si>
+  <si>
+    <t>R. Schaefer, J. Piggott</t>
+  </si>
+  <si>
+    <t>SETAC Rome</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Biodiversity and Ecosystem Functioning</t>
+  </si>
+  <si>
+    <t>Opinion</t>
+  </si>
+  <si>
+    <t>When things don't add up: quantifying impacts of multiple stressors from individual metabolism to ecosystem processing</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>N. Galic, L. Sullivan, V. Grimm, V. Forbes</t>
+  </si>
+  <si>
+    <t>What is synergy? The Saariselkä agreement revisited</t>
+  </si>
+  <si>
+    <t>Mini-review</t>
+  </si>
+  <si>
+    <t>Frontiers in Pharmacology</t>
+  </si>
+  <si>
+    <t>J. Tang, K. Wennerberg, T. Aittokallio</t>
+  </si>
+  <si>
+    <t>Interactions among ecosystem stressors and their importance in conservation</t>
+  </si>
+  <si>
+    <t>I. Cote, E. Darling, C. Brown</t>
+  </si>
+  <si>
+    <t>Proceedings of the Royal Society B</t>
+  </si>
+  <si>
+    <t>Analysing the impact of multiple stressors in aquatic biomonitoring data: A ‘cookbook’ with applications in R</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Science of the Total Enviroment</t>
+  </si>
+  <si>
+    <t>C. Feld, P. Segurado, C. Guttierez-Canovas</t>
+  </si>
+  <si>
+    <t>Additive effects prevail: The response of biota to multiple stressors in an intensively monitored watershed</t>
+  </si>
+  <si>
+    <t>Study, Field</t>
+  </si>
+  <si>
+    <t>A. Gieswein, D. Hering, C. Feld</t>
+  </si>
+  <si>
+    <t>Generalized concentration addition approach for predicting mixture toxicity</t>
+  </si>
+  <si>
+    <t>Enviromental Toxicology and Chemistry</t>
+  </si>
+  <si>
+    <t>Y. Tanaka, M. Tada</t>
   </si>
 </sst>
 </file>
@@ -120,13 +322,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1792,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB62B3D-6049-438B-9FF7-BB33F44B353D}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1887,4 +2092,455 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A814BDB0-CBF5-4F93-8A59-FDCA3CFD478B}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="76.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6">
+        <v>41913</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7">
+        <v>43251</v>
+      </c>
+      <c r="H2" s="7">
+        <v>43251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42064</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7">
+        <v>43255</v>
+      </c>
+      <c r="H3" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6">
+        <v>36100</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6">
+        <v>36281</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6">
+        <v>39753</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6">
+        <v>42370</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="6">
+        <v>41791</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="6">
+        <v>41791</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6">
+        <v>40969</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6">
+        <v>42186</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6">
+        <v>42675</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="6">
+        <v>43101</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="6">
+        <v>43132</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42248</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="6">
+        <v>42401</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6">
+        <v>42705</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="6">
+        <v>42979</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="6">
+        <v>42491</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added papers to tracker, updated stressor table, added isolate spreadsheet
</commit_message>
<xml_diff>
--- a/Writing Progress Tracker.xlsx
+++ b/Writing Progress Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC459FED-A288-4769-8D33-D5AFBF1F1071}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC04F51-CAAC-423A-816D-C486C0F0B01F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" activeTab="2" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
   <si>
     <t>Day</t>
   </si>
@@ -255,6 +255,42 @@
   </si>
   <si>
     <t>Y. Tanaka, M. Tada</t>
+  </si>
+  <si>
+    <t>Mixtures of Chemical Pollutants at European Legislation Safety Concentrations: How Safe Are They? </t>
+  </si>
+  <si>
+    <t>Carvalho et al.</t>
+  </si>
+  <si>
+    <t>Toxicological Sciences</t>
+  </si>
+  <si>
+    <t>C. Ritz, J. Streiberg</t>
+  </si>
+  <si>
+    <t>From additivity to synergism – A modelling perspective</t>
+  </si>
+  <si>
+    <t>Synergy</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Mechanisms of nickel toxicity in microorganisms.</t>
+  </si>
+  <si>
+    <t>L. Macomber, R. Hausinger</t>
+  </si>
+  <si>
+    <t>Metallomics</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Review of the molluscicide metaldehyde in the environment</t>
   </si>
 </sst>
 </file>
@@ -1995,6 +2031,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB62B3D-6049-438B-9FF7-BB33F44B353D}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2081,6 +2118,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12557BC7-E9BB-4FF3-ACB5-C0458929F97B}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2096,10 +2134,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A814BDB0-CBF5-4F93-8A59-FDCA3CFD478B}">
-  <dimension ref="A1:H19"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,10 +2146,11 @@
     <col min="1" max="1" width="76.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2172,7 +2212,9 @@
       <c r="B3" s="6">
         <v>42064</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
@@ -2196,7 +2238,9 @@
       <c r="B4" s="6">
         <v>36100</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
@@ -2207,6 +2251,9 @@
         <v>19</v>
       </c>
       <c r="G4" s="7">
+        <v>43255</v>
+      </c>
+      <c r="H4" s="7">
         <v>43255</v>
       </c>
     </row>
@@ -2217,7 +2264,9 @@
       <c r="B5" s="6">
         <v>36281</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
@@ -2228,6 +2277,9 @@
         <v>19</v>
       </c>
       <c r="G5" s="7">
+        <v>43255</v>
+      </c>
+      <c r="H5" s="7">
         <v>43255</v>
       </c>
     </row>
@@ -2537,6 +2589,80 @@
       </c>
       <c r="G19" s="7">
         <v>43255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="6">
+        <v>41883</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="6">
+        <v>41883</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="7">
+        <v>43255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="6">
+        <v>40848</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="7">
+        <v>43256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="7">
+        <v>43256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds Tom's modifications to robot script
</commit_message>
<xml_diff>
--- a/Writing Progress Tracker.xlsx
+++ b/Writing Progress Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC04F51-CAAC-423A-816D-C486C0F0B01F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B80C9-0EE6-40AC-ADB4-3C325F48D9A1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="7515" activeTab="2" xr2:uid="{A4221BD9-09B7-43DB-A191-43FE5C79320E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
   <si>
     <t>Day</t>
   </si>
@@ -291,6 +291,45 @@
   </si>
   <si>
     <t>Review of the molluscicide metaldehyde in the environment</t>
+  </si>
+  <si>
+    <t>Predictive environmental risk assessment of chemical mixtures: A conceptual framework</t>
+  </si>
+  <si>
+    <t>How well can we predict the toxicity of pesticide mixtures to aquatic life?</t>
+  </si>
+  <si>
+    <t>Quantifying Synergy: A Systematic Review of Mixture Toxicity Studies within Environmental Toxicology</t>
+  </si>
+  <si>
+    <t>Rethinking our approach to multiple stressor studies in marine environments</t>
+  </si>
+  <si>
+    <t>Density dependence governs when population responses to multiple stressors are magnified or mitigated</t>
+  </si>
+  <si>
+    <t>Interactions between effects of environmental chemicals and natural stressors: A review</t>
+  </si>
+  <si>
+    <t>Generalized concentration addition: A method for examining mixtures containing partial agonists</t>
+  </si>
+  <si>
+    <t>Predicting the synergy of multiple stress effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reconceptualizing synergism and antagonism among multiple stressors </t>
+  </si>
+  <si>
+    <t>Dose-Response Analysis Using R</t>
+  </si>
+  <si>
+    <t>Contribution of organic toxicants to multiple stress in river ecosystems</t>
+  </si>
+  <si>
+    <t>An improved null model for assessing the net effects of multiple stressors on communities</t>
+  </si>
+  <si>
+    <t>Impacts of multiple stressors on biodiversity and ecosystem functioning: the role of species co‐tolerance</t>
   </si>
 </sst>
 </file>
@@ -2135,10 +2174,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A814BDB0-CBF5-4F93-8A59-FDCA3CFD478B}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,6 +2491,9 @@
       <c r="G13" s="7">
         <v>43255</v>
       </c>
+      <c r="H13" s="7">
+        <v>43266</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2663,6 +2705,163 @@
       </c>
       <c r="G23" s="7">
         <v>43256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2012</v>
+      </c>
+      <c r="F24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="7">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="7">
+        <v>43266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>